<commit_message>
Scenario Manager | Solver | Week 5 Final Assessment
</commit_message>
<xml_diff>
--- a/Intermediate II/Week 5/workbook/W5_V4 ScenarioManager.xlsx
+++ b/Intermediate II/Week 5/workbook/W5_V4 ScenarioManager.xlsx
@@ -1,80 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nic\Documents\Freelance Training\Maquarie Uni\MOOCS\Course3\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foongmin\Desktop\excel-skills-for-business\Intermediate II\Week 5\workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A012AC82-E903-4209-A7CA-69F5F0BD850E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9163" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9130" yWindow="310" windowWidth="10070" windowHeight="9490" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projections &amp; Estimates" sheetId="3" r:id="rId1"/>
-    <sheet name="Project Costing Model" sheetId="1" r:id="rId2"/>
+    <sheet name="Scenario Summary" sheetId="4" r:id="rId2"/>
+    <sheet name="Project Costing Model" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="Quantity_Sold__Per_Manual">'Project Costing Model'!$E$16</definedName>
     <definedName name="Reviewers">'Projections &amp; Estimates'!#REF!</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Project Costing Model'!$B$7,'Project Costing Model'!$B$8,'Project Costing Model'!$B$9,'Project Costing Model'!$B$5</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Project Costing Model'!$B$7</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Project Costing Model'!$B$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Project Costing Model'!$B$8</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Project Costing Model'!$B$9</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Project Costing Model'!$B$9</definedName>
-    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Project Costing Model'!$E$7</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">6</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Project Costing Model'!$E$20</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel6" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">12</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">8</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">5</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">6</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">5</definedName>
-    <definedName name="solver_rhs6" localSheetId="1" hidden="1">24</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">24</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="Sale_Price">'Project Costing Model'!$E$15</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Project Costing Model'!$B$7,'Project Costing Model'!$B$8,'Project Costing Model'!$B$9,'Project Costing Model'!$B$5</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Project Costing Model'!$B$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Project Costing Model'!$B$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Project Costing Model'!$B$8</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Project Costing Model'!$B$9</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Project Costing Model'!$B$9</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">'Project Costing Model'!$E$7</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">6</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Project Costing Model'!$E$20</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">12</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">8</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">6</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">24</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">24</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>Total effort (hours)</t>
   </si>
@@ -233,6 +245,48 @@
   </si>
   <si>
     <t>Tasks &gt;= 100</t>
+  </si>
+  <si>
+    <t>Sale_Price</t>
+  </si>
+  <si>
+    <t>Quantity_Sold__Per_Manual</t>
+  </si>
+  <si>
+    <t>$E$20</t>
+  </si>
+  <si>
+    <t>Current Price</t>
+  </si>
+  <si>
+    <t>Created by Foong Min Wong on 29/6/2020</t>
+  </si>
+  <si>
+    <t>Price Decrease</t>
+  </si>
+  <si>
+    <t>Price Increase</t>
+  </si>
+  <si>
+    <t>Scenario Summary</t>
+  </si>
+  <si>
+    <t>Changing Cells:</t>
+  </si>
+  <si>
+    <t>Current Values:</t>
+  </si>
+  <si>
+    <t>Result Cells:</t>
+  </si>
+  <si>
+    <t>Notes:  Current Values column represents values of changing cells at</t>
+  </si>
+  <si>
+    <t>time Scenario Summary Report was created.  Changing cells for each</t>
+  </si>
+  <si>
+    <t>scenario are highlighted in gray.</t>
   </si>
 </sst>
 </file>
@@ -240,13 +294,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,8 +515,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,8 +739,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -770,6 +873,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -777,11 +918,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -822,20 +963,20 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -884,16 +1025,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="11" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="33" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="1" fillId="19" borderId="0" xfId="34" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="33"/>
     <xf numFmtId="165" fontId="1" fillId="19" borderId="0" xfId="34" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="33"/>
-    <xf numFmtId="164" fontId="1" fillId="19" borderId="0" xfId="34" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="19" borderId="0" xfId="34" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -908,10 +1049,41 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="34" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="27" builtinId="30" customBuiltin="1"/>
@@ -1276,22 +1448,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.4609375" customWidth="1"/>
-    <col min="2" max="3" width="18.4609375" customWidth="1"/>
-    <col min="4" max="4" width="19.61328125" customWidth="1"/>
-    <col min="5" max="5" width="18.4609375" customWidth="1"/>
-    <col min="6" max="6" width="17.3828125" customWidth="1"/>
-    <col min="7" max="7" width="20.921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.3828125" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+    <col min="2" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" customWidth="1"/>
+    <col min="7" max="7" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="35" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="35" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
@@ -1303,7 +1475,7 @@
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" s="35" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" s="35" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1313,7 +1485,7 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" s="26">
         <v>1</v>
       </c>
@@ -1327,7 +1499,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
         <v>34</v>
       </c>
@@ -1347,7 +1519,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
         <v>25</v>
       </c>
@@ -1369,7 +1541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1560,7 @@
       </c>
       <c r="F7" s="35"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
         <v>30</v>
       </c>
@@ -1407,7 +1579,7 @@
       </c>
       <c r="F8" s="35"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
         <v>27</v>
       </c>
@@ -1426,7 +1598,7 @@
       </c>
       <c r="F9" s="35"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
         <v>28</v>
       </c>
@@ -1445,7 +1617,7 @@
       </c>
       <c r="F10" s="35"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>29</v>
       </c>
@@ -1464,7 +1636,7 @@
       </c>
       <c r="F11" s="35"/>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="22" t="s">
         <v>31</v>
       </c>
@@ -1477,7 +1649,7 @@
       </c>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A13" s="35"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -1485,13 +1657,13 @@
       <c r="E13" s="35"/>
       <c r="F13" s="31"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
         <v>39</v>
       </c>
@@ -1506,7 +1678,7 @@
       <c r="E15" s="37"/>
       <c r="F15" s="31"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="36">
         <v>0.05</v>
       </c>
@@ -1523,7 +1695,7 @@
       </c>
       <c r="F16" s="31"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="36">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -1539,7 +1711,7 @@
       </c>
       <c r="F17" s="31"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="36">
         <v>0.08</v>
       </c>
@@ -1549,7 +1721,7 @@
       <c r="C18" s="31"/>
       <c r="F18" s="31"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="36">
         <v>9.5000000000000001E-2</v>
       </c>
@@ -1559,7 +1731,7 @@
       <c r="C19" s="31"/>
       <c r="F19" s="31"/>
     </row>
-    <row r="20" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="36">
         <v>0.11</v>
       </c>
@@ -1575,7 +1747,7 @@
       <c r="G20"/>
       <c r="H20" s="31"/>
     </row>
-    <row r="21" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="36">
         <v>0.125</v>
       </c>
@@ -1593,7 +1765,7 @@
       <c r="G21"/>
       <c r="H21" s="31"/>
     </row>
-    <row r="22" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="36">
         <v>0.14000000000000001</v>
       </c>
@@ -1611,7 +1783,7 @@
       <c r="G22"/>
       <c r="H22" s="31"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="36">
         <v>0.155</v>
       </c>
@@ -1625,7 +1797,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="33" t="s">
         <v>36</v>
       </c>
@@ -1637,7 +1809,7 @@
       <c r="G25" s="37"/>
       <c r="H25" s="37"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="32">
         <f>E21*E22*(1+E23)</f>
         <v>176015</v>
@@ -1670,7 +1842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="39">
         <v>0.03</v>
       </c>
@@ -1697,7 +1869,7 @@
         <v>217845</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="39">
         <v>0.04</v>
       </c>
@@ -1723,7 +1895,7 @@
         <v>219960</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="39">
         <v>0.05</v>
       </c>
@@ -1749,7 +1921,7 @@
         <v>222075</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="39">
         <v>0.06</v>
       </c>
@@ -1775,7 +1947,7 @@
         <v>224190</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="39">
         <v>0.08</v>
       </c>
@@ -1801,7 +1973,7 @@
         <v>228420.00000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="39">
         <v>0.09</v>
       </c>
@@ -1827,7 +1999,7 @@
         <v>230535.00000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="39">
         <v>0.1</v>
       </c>
@@ -1853,7 +2025,7 @@
         <v>232650.00000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="39">
         <v>0.11</v>
       </c>
@@ -1885,24 +2057,174 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36DD63D-EA08-4D29-B784-ADC25BEBEC1B}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:G12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.54296875" bestFit="1" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.5" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="31.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="63" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="57"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+    </row>
+    <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="56"/>
+      <c r="C6" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="50">
+        <v>35</v>
+      </c>
+      <c r="E6" s="61">
+        <v>35</v>
+      </c>
+      <c r="F6" s="61">
+        <v>30</v>
+      </c>
+      <c r="G6" s="61">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="56"/>
+      <c r="C7" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="51">
+        <v>2140</v>
+      </c>
+      <c r="E7" s="62">
+        <v>2140</v>
+      </c>
+      <c r="F7" s="62">
+        <v>2461</v>
+      </c>
+      <c r="G7" s="62">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+    </row>
+    <row r="9" spans="2:7" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="58"/>
+      <c r="C9" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="52">
+        <v>80000.000000000102</v>
+      </c>
+      <c r="E9" s="52">
+        <v>80000.000000000102</v>
+      </c>
+      <c r="F9" s="52">
+        <v>67594.202898550895</v>
+      </c>
+      <c r="G9" s="52">
+        <v>55188.405797101499</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.61328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.61328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.07421875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.61328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.61328125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.921875" style="1"/>
+    <col min="1" max="1" width="40.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="16" customFormat="1" ht="40.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
@@ -1912,7 +2234,7 @@
       <c r="E1" s="14"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:6" s="18" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" s="18" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -1920,7 +2242,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1928,7 +2250,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -1940,7 +2262,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>49</v>
       </c>
@@ -1957,7 +2279,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1974,7 +2296,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
@@ -1991,7 +2313,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -2003,7 +2325,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -2017,7 +2339,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -2034,7 +2356,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2051,7 +2373,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -2068,13 +2390,13 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -2084,7 +2406,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -2101,7 +2423,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -2118,7 +2440,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -2136,7 +2458,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -2153,7 +2475,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="8"/>
       <c r="C19" s="4"/>
@@ -2161,7 +2483,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2179,37 +2501,37 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2218,6 +2540,12 @@
       <c r="F26" s="4"/>
     </row>
   </sheetData>
+  <scenarios current="0" sqref="E20">
+    <scenario name="Price Increase" locked="1" count="2" user="Foong Min Wong" comment="Created by Foong Min Wong on 29/6/2020">
+      <inputCells r="E15" val="40" numFmtId="165"/>
+      <inputCells r="E16" val="1819" numFmtId="167"/>
+    </scenario>
+  </scenarios>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>